<commit_message>
Back to big images
</commit_message>
<xml_diff>
--- a/assignment_2/plots/Benchmarks.xlsx
+++ b/assignment_2/plots/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/University/4th Semester/Seminar/seminar_assignments/assignment_2/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF081D3-55BC-4A4B-BFE8-2C5CADA86873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF5FFEB-EC4C-CB4A-883A-EB44B9829233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19100" yWindow="500" windowWidth="18940" windowHeight="26580" xr2:uid="{5771DCD5-F8DD-A44A-92A6-DCFD402B2810}"/>
+    <workbookView xWindow="34480" yWindow="500" windowWidth="34300" windowHeight="26580" activeTab="1" xr2:uid="{5771DCD5-F8DD-A44A-92A6-DCFD402B2810}"/>
   </bookViews>
   <sheets>
     <sheet name="Phoenix" sheetId="1" r:id="rId1"/>
@@ -725,7 +725,7 @@
               <a:rPr lang="en-GB" sz="1600" baseline="0">
                 <a:latin typeface="+mj-lt"/>
               </a:rPr>
-              <a:t> Cache-Misses (Small Dataset)</a:t>
+              <a:t> Cache-Misses (Large Dataset)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1600">
               <a:latin typeface="+mj-lt"/>
@@ -13899,7 +13899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6F77C4-533C-A449-8C39-DB0FC58AEF38}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -15584,8 +15584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751D347C-B34A-D94E-A8C2-EFF493D9A06D}">
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added description in readme
</commit_message>
<xml_diff>
--- a/assignment_2/plots/Benchmarks.xlsx
+++ b/assignment_2/plots/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/University/4th Semester/Seminar/seminar_assignments/assignment_2/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D60EFA-127C-DA43-B04C-5B79130D243E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE820B2-5724-D440-B219-3C2B67A1296F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34480" yWindow="500" windowWidth="34300" windowHeight="26580" xr2:uid="{5771DCD5-F8DD-A44A-92A6-DCFD402B2810}"/>
+    <workbookView xWindow="22600" yWindow="500" windowWidth="22440" windowHeight="26580" activeTab="1" xr2:uid="{5771DCD5-F8DD-A44A-92A6-DCFD402B2810}"/>
   </bookViews>
   <sheets>
     <sheet name="Phoenix" sheetId="1" r:id="rId1"/>
@@ -3940,7 +3940,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Speed-Up (Small Dataset)</a:t>
+              <a:t> Speedup (Small Dataset)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -4395,7 +4395,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Speed-Up (Large Dataset)</a:t>
+              <a:t> Speedup (Large Dataset)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -13899,7 +13899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6F77C4-533C-A449-8C39-DB0FC58AEF38}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D2" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -15584,8 +15584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751D347C-B34A-D94E-A8C2-EFF493D9A06D}">
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>